<commit_message>
Fixed Transformer and List Initializations
Changed the Transformer class to have an input member and to store its
products and product efficiencies in a dictionary. Also fixed the four
main lists to initialize them to their respective classes
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -65,6 +65,12 @@
   </si>
   <si>
     <t>EnergyType</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>etc</t>
   </si>
 </sst>
 </file>
@@ -464,44 +470,50 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" t="s">
-        <v>2</v>
+      <c r="L1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -513,7 +525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Almost finished object initialization
For all except transformers, the object-list initialization is done. The
transformers still need a dynamic way to set up the dictionary holding
their product and efficency values, but I'll do that later. It should be
easy. Keyword being should.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -411,7 +411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -441,7 +441,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
@@ -449,7 +449,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,9 +457,12 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -525,7 +528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated Input Data File
The input data spreadsheet now has the data for the first test case
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -17,23 +17,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Capex</t>
-  </si>
-  <si>
-    <t>Opex</t>
-  </si>
-  <si>
-    <t>CO2</t>
-  </si>
-  <si>
-    <t>Demand</t>
-  </si>
-  <si>
     <t>TotalEff</t>
   </si>
   <si>
@@ -55,9 +43,6 @@
     <t>SubEff3</t>
   </si>
   <si>
-    <t xml:space="preserve"> Capex</t>
-  </si>
-  <si>
     <t>In</t>
   </si>
   <si>
@@ -71,6 +56,57 @@
   </si>
   <si>
     <t>etc</t>
+  </si>
+  <si>
+    <t>CrOil</t>
+  </si>
+  <si>
+    <t>crudeOil</t>
+  </si>
+  <si>
+    <t>CO2 in kg/MJ</t>
+  </si>
+  <si>
+    <t>Capex in $</t>
+  </si>
+  <si>
+    <t>Opex in $/MJ</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>hydrogen</t>
+  </si>
+  <si>
+    <t>Gasoline</t>
+  </si>
+  <si>
+    <t>Demand in MJ</t>
+  </si>
+  <si>
+    <t>gasoline</t>
+  </si>
+  <si>
+    <t>Refinery</t>
+  </si>
+  <si>
+    <t>crudeoil</t>
+  </si>
+  <si>
+    <t>MtG</t>
+  </si>
+  <si>
+    <t>cr2ref</t>
+  </si>
+  <si>
+    <t>h22mtg</t>
+  </si>
+  <si>
+    <t>ref2gas</t>
+  </si>
+  <si>
+    <t>mtg2gas</t>
   </si>
 </sst>
 </file>
@@ -409,29 +445,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0.01</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2">
+        <v>7.3200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0.05</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -441,29 +518,53 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -473,50 +574,110 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" t="s">
-        <v>17</v>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0.93</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0.84</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -526,10 +687,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,13 +700,69 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Friday Start, File Reading Almost Done
Testing something with git, and committing the nearly-done file reading
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>Input</t>
-  </si>
-  <si>
-    <t>etc</t>
   </si>
   <si>
     <t>CrOil</t>
@@ -465,21 +462,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
         <v>16</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
       </c>
       <c r="D1" t="s">
         <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -488,7 +485,7 @@
         <v>0.01</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2">
         <v>7.3200000000000001E-2</v>
@@ -496,7 +493,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -505,7 +502,7 @@
         <v>0.05</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -538,21 +535,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
         <v>16</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
       </c>
       <c r="D1" t="s">
         <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -561,7 +558,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2">
         <v>1000</v>
@@ -574,10 +571,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,7 +593,7 @@
     <col min="12" max="12" width="3.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -604,10 +601,10 @@
         <v>11</v>
       </c>
       <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
         <v>16</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -630,16 +627,13 @@
       <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
         <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -651,18 +645,18 @@
         <v>0.93</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -674,7 +668,7 @@
         <v>0.84</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -689,7 +683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -711,58 +705,58 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
         <v>23</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
         <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed excel units again
Turns out moving the units down the column screwed up the indexing.
Fixed it by changing the units to be a comment on the cell that they
apply to. Please use this convention if you add any more qualities.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -16,8 +16,237 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+in $
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+in $ per MJ
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+in kg/MJ</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+in $
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+in $/MJ
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+in MJ
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+in $
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+in $/MJ
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
@@ -97,25 +326,7 @@
     <t>CO2</t>
   </si>
   <si>
-    <t>in $</t>
-  </si>
-  <si>
-    <t>in $ per MJ</t>
-  </si>
-  <si>
-    <t>in kg/MJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> in $</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> in $/MJ</t>
-  </si>
-  <si>
     <t>Demand</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> in MJ</t>
   </si>
   <si>
     <t>Prod0</t>
@@ -128,13 +339,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -459,11 +683,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,28 +750,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" t="s">
-        <v>28</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,7 +787,7 @@
         <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -593,28 +807,18 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" t="s">
-        <v>32</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,10 +854,10 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
@@ -714,16 +918,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" t="s">
-        <v>30</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -731,7 +928,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Reading almost done for real now
It's actually almost done. Also I think I fixed something in the input
sheet, but I'm not sure.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -246,7 +246,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -333,6 +333,15 @@
   </si>
   <si>
     <t>SubEff0</t>
+  </si>
+  <si>
+    <t>jetfuel</t>
+  </si>
+  <si>
+    <t>kerosene</t>
+  </si>
+  <si>
+    <t>STEVE-O</t>
   </si>
 </sst>
 </file>
@@ -815,24 +824,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -892,7 +901,19 @@
         <v>15</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0.5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2">
+        <v>0.3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2">
+        <v>0.2</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -916,6 +937,35 @@
       </c>
       <c r="G3">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0.95</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4">
+        <v>0.6</v>
+      </c>
+      <c r="H4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4">
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>
@@ -928,7 +978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Only commiting so I can pull, no changes
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -692,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,7 +840,12 @@
     <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated input for current test case
Removed our design test values from the input spreadsheet and replaced
them with correct test values for Max's test case
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -246,7 +246,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -330,15 +330,6 @@
   </si>
   <si>
     <t>SubEff0</t>
-  </si>
-  <si>
-    <t>jetfuel</t>
-  </si>
-  <si>
-    <t>kerosene</t>
-  </si>
-  <si>
-    <t>STEVE-O</t>
   </si>
 </sst>
 </file>
@@ -692,7 +683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
@@ -821,10 +812,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,19 +894,7 @@
         <v>14</v>
       </c>
       <c r="G2">
-        <v>0.5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2">
-        <v>0.3</v>
-      </c>
-      <c r="J2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -939,35 +918,6 @@
       </c>
       <c r="G3">
         <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0.95</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4">
-        <v>0.6</v>
-      </c>
-      <c r="H4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4">
-        <v>0.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Signed-off-by: Steven Witkin <switkin1@jhu.edu>
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -246,7 +246,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -330,48 +330,6 @@
   </si>
   <si>
     <t>SubEff0</t>
-  </si>
-  <si>
-    <t>S2</t>
-  </si>
-  <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t>water</t>
-  </si>
-  <si>
-    <t>methane</t>
-  </si>
-  <si>
-    <t>vibranium</t>
-  </si>
-  <si>
-    <t>wtg</t>
-  </si>
-  <si>
-    <t>meta</t>
-  </si>
-  <si>
-    <t>ref2vib</t>
-  </si>
-  <si>
-    <t>Vibranium</t>
-  </si>
-  <si>
-    <t>m2vib</t>
-  </si>
-  <si>
-    <t>s11</t>
-  </si>
-  <si>
-    <t>s22</t>
-  </si>
-  <si>
-    <t>s33</t>
-  </si>
-  <si>
-    <t>s44</t>
   </si>
 </sst>
 </file>
@@ -723,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,40 +747,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>1E-3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5">
-        <v>0.1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -831,10 +755,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,23 +804,6 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3">
-        <v>50</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -905,10 +812,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,13 +894,7 @@
         <v>14</v>
       </c>
       <c r="G2">
-        <v>0.95</v>
-      </c>
-      <c r="H2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2">
-        <v>0.05</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1017,58 +918,6 @@
       </c>
       <c r="G3">
         <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0.8</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5">
-        <v>0.5</v>
-      </c>
-      <c r="H5" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5">
-        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -1079,10 +928,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1160,90 +1009,6 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" t="s">
-        <v>14</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added basic hub capability
Added a sheet for resource hubs to the input and added a class for
resource hubs (AKA depots)
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
     <sheet name="Sinks" sheetId="2" r:id="rId2"/>
     <sheet name="Transformers" sheetId="3" r:id="rId3"/>
     <sheet name="Connectors" sheetId="4" r:id="rId4"/>
+    <sheet name="Hubs" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -246,7 +247,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
@@ -330,6 +331,9 @@
   </si>
   <si>
     <t>SubEff0</t>
+  </si>
+  <si>
+    <t>Energy Type</t>
   </si>
 </sst>
 </file>
@@ -814,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,4 +1016,33 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added capex functionality. still needs further testing/ examples
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -247,7 +247,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -288,9 +288,6 @@
     <t>hydrogen</t>
   </si>
   <si>
-    <t>Gasoline</t>
-  </si>
-  <si>
     <t>gasoline</t>
   </si>
   <si>
@@ -333,7 +330,43 @@
     <t>SubEff0</t>
   </si>
   <si>
-    <t>Energy Type</t>
+    <t>GasHub</t>
+  </si>
+  <si>
+    <t>KmHub</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>Gtkm</t>
+  </si>
+  <si>
+    <t>Kilometers</t>
+  </si>
+  <si>
+    <t>BM</t>
+  </si>
+  <si>
+    <t>biomass</t>
+  </si>
+  <si>
+    <t>B2gas</t>
+  </si>
+  <si>
+    <t>gas2km</t>
+  </si>
+  <si>
+    <t>kmtohub</t>
+  </si>
+  <si>
+    <t>hub2sink</t>
+  </si>
+  <si>
+    <t>bm2btg</t>
+  </si>
+  <si>
+    <t>btg2gas</t>
   </si>
 </sst>
 </file>
@@ -685,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,16 +738,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
         <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>23</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -728,7 +761,7 @@
         <v>0.01</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2">
         <v>7.3200000000000001E-2</v>
@@ -749,6 +782,23 @@
       </c>
       <c r="E3">
         <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0.02</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4">
+        <v>0.04</v>
       </c>
     </row>
   </sheetData>
@@ -762,7 +812,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,21 +829,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
         <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>23</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -802,7 +852,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="E2">
         <v>1000</v>
@@ -816,10 +866,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T20" sqref="T20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,19 +901,19 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
         <v>22</v>
-      </c>
-      <c r="D1" t="s">
-        <v>23</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
       </c>
       <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
         <v>26</v>
-      </c>
-      <c r="G1" t="s">
-        <v>27</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
@@ -880,13 +930,13 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
       <c r="C2">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -895,7 +945,7 @@
         <v>0.93</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -903,7 +953,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -918,9 +968,55 @@
         <v>0.84</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0.4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0.5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5">
         <v>1</v>
       </c>
     </row>
@@ -932,10 +1028,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,27 +1055,27 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
         <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -987,30 +1083,100 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
         <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
-        <v>14</v>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1020,10 +1186,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,13 +1199,41 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>28</v>
       </c>
-      <c r="C1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" t="s">
-        <v>23</v>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added multiple transformer inputs
Transformers can now take multiple inputs. Things aren't working, but
we're getting there. Also, there are now min and max values for sources.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -193,7 +193,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -218,7 +218,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -282,7 +282,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="42">
   <si>
     <t>Name</t>
   </si>
@@ -296,12 +296,6 @@
     <t>SubEff1</t>
   </si>
   <si>
-    <t>Prod2</t>
-  </si>
-  <si>
-    <t>SubEff2</t>
-  </si>
-  <si>
     <t>In</t>
   </si>
   <si>
@@ -311,9 +305,6 @@
     <t>EnergyType</t>
   </si>
   <si>
-    <t>Input</t>
-  </si>
-  <si>
     <t>CrOil</t>
   </si>
   <si>
@@ -405,6 +396,18 @@
   </si>
   <si>
     <t>CO2 Max</t>
+  </si>
+  <si>
+    <t>Input0</t>
+  </si>
+  <si>
+    <t>MinProduction</t>
+  </si>
+  <si>
+    <t>MaxProduction</t>
+  </si>
+  <si>
+    <t>InRatio0</t>
   </si>
 </sst>
 </file>
@@ -756,41 +759,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -799,15 +810,21 @@
         <v>0.01</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E2">
         <v>7.3200000000000001E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -816,15 +833,21 @@
         <v>0.05</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -833,10 +856,16 @@
         <v>0.02</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E4">
         <v>0.04</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>9999999</v>
       </c>
     </row>
   </sheetData>
@@ -867,21 +896,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
         <v>21</v>
-      </c>
-      <c r="C1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -890,7 +919,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E2">
         <v>1000</v>
@@ -904,157 +933,167 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0.93</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0.84</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F3">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0.4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
         <v>26</v>
       </c>
-      <c r="H1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2">
-        <v>200</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0.93</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2">
+      <c r="H4">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0.84</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0.5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0.4</v>
-      </c>
-      <c r="F4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0.5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5">
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5">
         <v>1</v>
       </c>
     </row>
@@ -1082,139 +1121,139 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
         <v>28</v>
       </c>
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1237,21 +1276,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1262,10 +1301,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1283,7 +1322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1291,7 +1330,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added transformer in ratio calculation
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -282,7 +282,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="44">
   <si>
     <t>Name</t>
   </si>
@@ -408,6 +408,12 @@
   </si>
   <si>
     <t>InRatio0</t>
+  </si>
+  <si>
+    <t>Input1</t>
+  </si>
+  <si>
+    <t>InRatio1</t>
   </si>
 </sst>
 </file>
@@ -933,10 +939,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,22 +952,22 @@
     <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9.42578125" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="9.42578125" customWidth="1"/>
+    <col min="11" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -981,19 +987,25 @@
         <v>41</v>
       </c>
       <c r="G1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>23</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1012,14 +1024,14 @@
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1038,14 +1050,14 @@
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>10</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1064,14 +1076,14 @@
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>26</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1090,10 +1102,10 @@
       <c r="F5">
         <v>1</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>10</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>1</v>
       </c>
     </row>
@@ -1108,7 +1120,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added full opex calculation.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -941,7 +941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -1277,8 +1277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added min and max ranges for opex and totalEff
In preparation for implementing the Monte Carlo method, opex and
totalEff values have been expanded to include averages, mins, and maxes
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -49,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -74,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -133,7 +133,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -158,7 +158,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -218,7 +218,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -282,14 +282,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>TotalEff</t>
-  </si>
-  <si>
     <t>Prod1</t>
   </si>
   <si>
@@ -341,9 +338,6 @@
     <t>Capex</t>
   </si>
   <si>
-    <t>Opex</t>
-  </si>
-  <si>
     <t>CO2</t>
   </si>
   <si>
@@ -414,6 +408,24 @@
   </si>
   <si>
     <t>InRatio1</t>
+  </si>
+  <si>
+    <t>OpexAvg</t>
+  </si>
+  <si>
+    <t>OpexMin</t>
+  </si>
+  <si>
+    <t>OpexMax</t>
+  </si>
+  <si>
+    <t>TotalEffMin</t>
+  </si>
+  <si>
+    <t>TotalEffAvg</t>
+  </si>
+  <si>
+    <t>TotalEffMax</t>
   </si>
 </sst>
 </file>
@@ -765,112 +777,138 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1E-3</v>
+      </c>
+      <c r="D2">
+        <v>0.01</v>
+      </c>
+      <c r="E2">
+        <v>0.1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2">
+        <v>7.3200000000000001E-2</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0.01</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2">
-        <v>7.3200000000000001E-2</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1E-3</v>
+      </c>
+      <c r="D3">
+        <v>0.05</v>
+      </c>
+      <c r="E3">
+        <v>0.1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
         <v>9999999</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0.05</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>9999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
+        <v>1E-3</v>
+      </c>
+      <c r="D4">
         <v>0.02</v>
       </c>
-      <c r="D4" t="s">
-        <v>30</v>
-      </c>
       <c r="E4">
+        <v>0.1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4">
         <v>0.04</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
         <v>9999999</v>
       </c>
     </row>
@@ -882,41 +920,49 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -924,10 +970,16 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
-        <v>26</v>
+      <c r="D2">
+        <v>0</v>
       </c>
       <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2">
         <v>1000</v>
       </c>
     </row>
@@ -939,101 +991,133 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="9.42578125" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="P1" t="s">
         <v>2</v>
       </c>
-      <c r="L1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0.8</v>
+      </c>
+      <c r="G2">
+        <v>0.93</v>
+      </c>
+      <c r="H2">
+        <v>0.95</v>
+      </c>
+      <c r="I2" t="s">
         <v>11</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0.93</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>10</v>
       </c>
       <c r="J2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1042,24 +1126,36 @@
         <v>0</v>
       </c>
       <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0.8</v>
+      </c>
+      <c r="G3">
         <v>0.84</v>
       </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
+      <c r="H3">
+        <v>0.9</v>
       </c>
       <c r="I3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1068,24 +1164,36 @@
         <v>0</v>
       </c>
       <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0.3</v>
+      </c>
+      <c r="G4">
         <v>0.4</v>
       </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
+      <c r="H4">
+        <v>0.5</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="J4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1094,18 +1202,30 @@
         <v>0</v>
       </c>
       <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0.3</v>
+      </c>
+      <c r="G5">
         <v>0.5</v>
       </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5">
+      <c r="H5">
+        <v>0.6</v>
+      </c>
+      <c r="I5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5">
         <v>1</v>
       </c>
-      <c r="I5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5">
+      <c r="M5" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5">
         <v>1</v>
       </c>
     </row>
@@ -1120,7 +1240,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1133,139 +1253,139 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
         <v>29</v>
       </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1275,53 +1395,71 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
         <v>0</v>
       </c>
     </row>
@@ -1342,7 +1480,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Monte Carlo Additions Underway
Work has begun on adding Monte Carlo simulation functionality to the
model.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -282,7 +282,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -426,6 +426,9 @@
   </si>
   <si>
     <t>TotalEffMax</t>
+  </si>
+  <si>
+    <t>NumIterations</t>
   </si>
 </sst>
 </file>
@@ -780,7 +783,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1397,7 +1400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -1470,22 +1473,32 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>40</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ability to set usage of a source.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -282,7 +282,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -392,12 +392,6 @@
     <t>Input0</t>
   </si>
   <si>
-    <t>MinProduction</t>
-  </si>
-  <si>
-    <t>MaxProduction</t>
-  </si>
-  <si>
     <t>InRatio0</t>
   </si>
   <si>
@@ -435,6 +429,18 @@
   </si>
   <si>
     <t>DemandMax</t>
+  </si>
+  <si>
+    <t>IsSet</t>
+  </si>
+  <si>
+    <t>UsageMin</t>
+  </si>
+  <si>
+    <t>UsageAvg</t>
+  </si>
+  <si>
+    <t>UsageMax</t>
   </si>
 </sst>
 </file>
@@ -786,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,7 +811,7 @@
     <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -813,13 +819,13 @@
         <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
         <v>41</v>
-      </c>
-      <c r="E1" t="s">
-        <v>43</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -828,13 +834,19 @@
         <v>18</v>
       </c>
       <c r="H1" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="I1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="J1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -857,13 +869,19 @@
         <v>7.3200000000000001E-2</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2">
-        <v>9999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+      <c r="J2">
+        <v>300</v>
+      </c>
+      <c r="K2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -889,10 +907,16 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>9999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -918,7 +942,13 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>9999999</v>
+        <v>10</v>
+      </c>
+      <c r="J4">
+        <v>660000</v>
+      </c>
+      <c r="K4">
+        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -931,7 +961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -955,25 +985,25 @@
         <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
         <v>41</v>
-      </c>
-      <c r="E1" t="s">
-        <v>43</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" t="s">
         <v>48</v>
-      </c>
-      <c r="I1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1057,34 +1087,34 @@
         <v>17</v>
       </c>
       <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
         <v>42</v>
       </c>
-      <c r="D1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>44</v>
-      </c>
-      <c r="G1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" t="s">
-        <v>46</v>
       </c>
       <c r="I1" t="s">
         <v>35</v>
       </c>
       <c r="J1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" t="s">
         <v>38</v>
-      </c>
-      <c r="K1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L1" t="s">
-        <v>40</v>
       </c>
       <c r="M1" t="s">
         <v>19</v>
@@ -1436,13 +1466,13 @@
         <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
         <v>41</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1509,7 +1539,7 @@
         <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added output for products of transformers
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -282,7 +282,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -441,6 +441,9 @@
   </si>
   <si>
     <t>UsageMax</t>
+  </si>
+  <si>
+    <t>ref2km</t>
   </si>
 </sst>
 </file>
@@ -794,7 +797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
@@ -1045,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,7 +1167,13 @@
         <v>9</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <v>0.999</v>
+      </c>
+      <c r="O2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -1207,7 +1216,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1225,19 +1234,19 @@
         <v>0.3</v>
       </c>
       <c r="G4">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="H4">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="I4" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="J4">
         <v>1</v>
       </c>
       <c r="M4" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="N4">
         <v>1</v>
@@ -1245,7 +1254,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1263,19 +1272,19 @@
         <v>0.3</v>
       </c>
       <c r="G5">
+        <v>0.4</v>
+      </c>
+      <c r="H5">
         <v>0.5</v>
       </c>
-      <c r="H5">
-        <v>0.6</v>
-      </c>
       <c r="I5" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="J5">
         <v>1</v>
       </c>
       <c r="M5" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="N5">
         <v>1</v>
@@ -1289,10 +1298,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1438,6 +1447,20 @@
       </c>
       <c r="D10" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gotta commit in order to pull
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -794,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,16 +869,16 @@
         <v>7.3200000000000001E-2</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="J2">
-        <v>300</v>
+        <v>2000</v>
       </c>
       <c r="K2">
-        <v>400</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -910,10 +910,10 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -939,16 +939,16 @@
         <v>0.04</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="J4">
-        <v>660000</v>
+        <v>4000</v>
       </c>
       <c r="K4">
-        <v>500</v>
+        <v>8000</v>
       </c>
     </row>
   </sheetData>
@@ -1524,8 +1524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1544,7 +1544,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>40</v>
+        <v>400</v>
       </c>
       <c r="B2">
         <v>10</v>

</xml_diff>

<commit_message>
added limits on transformers
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -282,7 +282,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -441,6 +441,12 @@
   </si>
   <si>
     <t>UsageMax</t>
+  </si>
+  <si>
+    <t>OutMin</t>
+  </si>
+  <si>
+    <t>OutMax</t>
   </si>
 </sst>
 </file>
@@ -795,7 +801,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,13 +913,13 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>2200</v>
       </c>
       <c r="J3">
-        <v>2000</v>
+        <v>2400</v>
       </c>
       <c r="K3">
-        <v>4000</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -939,7 +945,7 @@
         <v>0.04</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4">
         <v>1000</v>
@@ -1043,10 +1049,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,30 +1062,31 @@
     <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.42578125" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1096,40 +1103,46 @@
         <v>41</v>
       </c>
       <c r="F1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>43</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>44</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>35</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>36</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>37</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>38</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>19</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>1</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1146,28 +1159,34 @@
         <v>0</v>
       </c>
       <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>200</v>
+      </c>
+      <c r="H2">
         <v>0.8</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>0.93</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>0.95</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>11</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>1</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>9</v>
       </c>
-      <c r="N2">
+      <c r="P2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1184,28 +1203,34 @@
         <v>0</v>
       </c>
       <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>999999</v>
+      </c>
+      <c r="H3">
         <v>0.8</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>0.84</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>0.9</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>8</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>1</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>9</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -1222,28 +1247,34 @@
         <v>0</v>
       </c>
       <c r="F4">
+        <v>850</v>
+      </c>
+      <c r="G4">
+        <v>999999</v>
+      </c>
+      <c r="H4">
         <v>0.3</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>0.4</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>0.5</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>9</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>1</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>23</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1260,24 +1291,30 @@
         <v>0</v>
       </c>
       <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>999999</v>
+      </c>
+      <c r="H5">
         <v>0.3</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>0.5</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>0.6</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>27</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>1</v>
       </c>
-      <c r="M5" t="s">
+      <c r="O5" t="s">
         <v>9</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <v>1</v>
       </c>
     </row>
@@ -1524,7 +1561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Preparing to start gekko version
Commented out current implementation of check model, output, and a few
other things. This is just to set up for working on the new gekko
version of this project.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -1051,7 +1051,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1561,7 +1561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1581,7 +1581,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>40</v>
+        <v>4000</v>
       </c>
       <c r="B2">
         <v>10</v>

</xml_diff>

<commit_message>
Removed CO2Loc and Added Distribution Flexibility
Removed all code pertaining to CO2 locations hopefully, as it is no
longer used in this version. Also added the framework for eventually
using non-normal distributions by adding a distributions input into the
input sheet and adding some if statements to handle it. It can only
handle normal right now, but rayleigh will be added shortly.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" tabRatio="607"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -277,12 +277,38 @@
         </r>
       </text>
     </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Options for this are:
+normal
+..rayleigh..</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -320,21 +346,6 @@
     <t>crudeoil</t>
   </si>
   <si>
-    <t>MtG</t>
-  </si>
-  <si>
-    <t>cr2ref</t>
-  </si>
-  <si>
-    <t>h22mtg</t>
-  </si>
-  <si>
-    <t>ref2gas</t>
-  </si>
-  <si>
-    <t>mtg2gas</t>
-  </si>
-  <si>
     <t>Capex</t>
   </si>
   <si>
@@ -347,45 +358,12 @@
     <t>SubEff0</t>
   </si>
   <si>
-    <t>GasHub</t>
-  </si>
-  <si>
-    <t>KmHub</t>
-  </si>
-  <si>
-    <t>km</t>
-  </si>
-  <si>
-    <t>Gtkm</t>
-  </si>
-  <si>
-    <t>Kilometers</t>
-  </si>
-  <si>
     <t>BM</t>
   </si>
   <si>
     <t>biomass</t>
   </si>
   <si>
-    <t>B2gas</t>
-  </si>
-  <si>
-    <t>gas2km</t>
-  </si>
-  <si>
-    <t>kmtohub</t>
-  </si>
-  <si>
-    <t>hub2sink</t>
-  </si>
-  <si>
-    <t>bm2btg</t>
-  </si>
-  <si>
-    <t>btg2gas</t>
-  </si>
-  <si>
     <t>CO2 Max</t>
   </si>
   <si>
@@ -447,6 +425,102 @@
   </si>
   <si>
     <t>OutMax</t>
+  </si>
+  <si>
+    <t>pkm</t>
+  </si>
+  <si>
+    <t>tkm-N1</t>
+  </si>
+  <si>
+    <t>tkm</t>
+  </si>
+  <si>
+    <t>tkm-N2</t>
+  </si>
+  <si>
+    <t>tkm-N3</t>
+  </si>
+  <si>
+    <t>tkm-SZM</t>
+  </si>
+  <si>
+    <t>BtL</t>
+  </si>
+  <si>
+    <t>PtF</t>
+  </si>
+  <si>
+    <t>PVGas</t>
+  </si>
+  <si>
+    <t>TruckN1</t>
+  </si>
+  <si>
+    <t>TruckN2</t>
+  </si>
+  <si>
+    <t>TruckN3</t>
+  </si>
+  <si>
+    <t>TruckSZM</t>
+  </si>
+  <si>
+    <t>1-cr</t>
+  </si>
+  <si>
+    <t>1-bm_1</t>
+  </si>
+  <si>
+    <t>1-h2_1</t>
+  </si>
+  <si>
+    <t>2-cr_gas</t>
+  </si>
+  <si>
+    <t>GasolineHub</t>
+  </si>
+  <si>
+    <t>2-btl</t>
+  </si>
+  <si>
+    <t>2-h2_1</t>
+  </si>
+  <si>
+    <t>3-gas_PV</t>
+  </si>
+  <si>
+    <t>3-TrN1</t>
+  </si>
+  <si>
+    <t>3-TrN2</t>
+  </si>
+  <si>
+    <t>3-TrN3</t>
+  </si>
+  <si>
+    <t>3-TrSZM</t>
+  </si>
+  <si>
+    <t>4-gasPV</t>
+  </si>
+  <si>
+    <t>4-TrN1</t>
+  </si>
+  <si>
+    <t>4-TrN2</t>
+  </si>
+  <si>
+    <t>4-TrN3</t>
+  </si>
+  <si>
+    <t>4-TrSZM</t>
+  </si>
+  <si>
+    <t>Distribution</t>
+  </si>
+  <si>
+    <t>normal</t>
   </si>
 </sst>
 </file>
@@ -495,8 +569,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,34 +898,34 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H1" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="I1" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="J1" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="K1" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -860,13 +936,13 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="D2">
-        <v>0.01</v>
+        <v>1.2E-2</v>
       </c>
       <c r="E2">
-        <v>0.1</v>
+        <v>0.04</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -878,83 +954,83 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>4000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>1E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D3">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="E3">
-        <v>0.1</v>
+        <v>0.03</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>2200</v>
+        <v>300</v>
       </c>
       <c r="J3">
-        <v>2400</v>
+        <v>400</v>
       </c>
       <c r="K3">
-        <v>2600</v>
+        <v>500</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>1E-3</v>
+        <v>0.04</v>
       </c>
       <c r="D4">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="E4">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="G4">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>8000</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -965,10 +1041,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,33 +1064,33 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="H1" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="I1" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1029,16 +1105,132 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="G2">
-        <v>950</v>
+        <v>700</v>
       </c>
       <c r="H2">
+        <v>858</v>
+      </c>
+      <c r="I2">
         <v>1000</v>
       </c>
-      <c r="I2">
-        <v>1050</v>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>7.5</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4">
+        <v>20</v>
+      </c>
+      <c r="H4">
+        <v>24.2</v>
+      </c>
+      <c r="I4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5">
+        <v>110</v>
+      </c>
+      <c r="H5">
+        <v>130.30000000000001</v>
+      </c>
+      <c r="I5">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6">
+        <v>350</v>
+      </c>
+      <c r="H6">
+        <v>414.5</v>
+      </c>
+      <c r="I6">
+        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -1049,10 +1241,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1091,49 +1283,49 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="G1" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="H1" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="I1" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="J1" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="K1" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="L1" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="M1" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="N1" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="O1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="Q1" t="s">
         <v>1</v>
@@ -1150,28 +1342,28 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>200</v>
-      </c>
-      <c r="H2">
-        <v>0.8</v>
-      </c>
-      <c r="I2">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>999999</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="I2" s="2">
         <v>0.93</v>
       </c>
-      <c r="J2">
-        <v>0.95</v>
+      <c r="J2" s="1">
+        <v>0.94</v>
       </c>
       <c r="K2" t="s">
         <v>11</v>
@@ -1188,37 +1380,37 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
         <v>999999</v>
       </c>
-      <c r="H3">
-        <v>0.8</v>
-      </c>
-      <c r="I3">
-        <v>0.84</v>
-      </c>
-      <c r="J3">
-        <v>0.9</v>
+      <c r="H3" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.54</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.6</v>
       </c>
       <c r="K3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -1232,43 +1424,43 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>850</v>
-      </c>
-      <c r="G4">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
         <v>999999</v>
       </c>
-      <c r="H4">
-        <v>0.3</v>
-      </c>
-      <c r="I4">
-        <v>0.4</v>
-      </c>
-      <c r="J4">
-        <v>0.5</v>
+      <c r="H4" s="1">
+        <v>0.76</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.84</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.86</v>
       </c>
       <c r="K4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L4">
         <v>1</v>
       </c>
       <c r="O4" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="P4">
         <v>1</v>
@@ -1276,45 +1468,221 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
         <v>999999</v>
       </c>
-      <c r="H5">
-        <v>0.3</v>
-      </c>
-      <c r="I5">
-        <v>0.5</v>
-      </c>
-      <c r="J5">
-        <v>0.6</v>
+      <c r="H5" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.78947368421052633</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.85</v>
       </c>
       <c r="K5" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="L5">
         <v>1</v>
       </c>
       <c r="O5" t="s">
+        <v>39</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="D6">
+        <v>1E-3</v>
+      </c>
+      <c r="E6">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>999999</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="I6" s="2">
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K6" t="s">
         <v>9</v>
       </c>
-      <c r="P5">
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="O6" t="s">
+        <v>41</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="D7">
+        <v>1E-3</v>
+      </c>
+      <c r="E7">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>999999</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.6923076923076924</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="K7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="O7" t="s">
+        <v>41</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="D8">
+        <v>1E-3</v>
+      </c>
+      <c r="E8">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>999999</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.70512820512820518</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="K8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="O8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="D9">
+        <v>1E-3</v>
+      </c>
+      <c r="E9">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>999999</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I9" s="2">
+        <v>1.5340909090909089</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="K9" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="O9" t="s">
+        <v>41</v>
+      </c>
+      <c r="P9">
         <v>1</v>
       </c>
     </row>
@@ -1326,10 +1694,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1353,7 +1721,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -1367,41 +1735,41 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -1409,13 +1777,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -1423,58 +1791,156 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1484,10 +1950,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1500,21 +1966,21 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -1523,33 +1989,13 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
+        <v>1.1000000000000001E-3</v>
       </c>
     </row>
   </sheetData>
@@ -1559,10 +2005,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1571,20 +2017,26 @@
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>40</v>
+        <v>87.213999999999999</v>
       </c>
       <c r="B2">
         <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Dynamic Distribution Selection
Added bounds, so that if a given average is within 10% of the midpoint,
the normal distribution will be automatically selected. Also refined the
rayleigh distribution implementation to improve the switching of which
side is biased.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -32,7 +32,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -41,7 +41,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 in $
@@ -57,7 +57,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -66,7 +66,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 in $ per MJ
@@ -82,7 +82,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -91,7 +91,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 in kg/MJ</t>
@@ -116,7 +116,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -125,7 +125,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 in $
@@ -141,7 +141,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -150,7 +150,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 in $/MJ
@@ -166,7 +166,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -175,7 +175,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 in MJ
@@ -201,7 +201,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -210,7 +210,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 in $
@@ -226,7 +226,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -235,7 +235,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 in $/MJ
@@ -261,7 +261,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -270,7 +270,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 in kg</t>
@@ -285,7 +285,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -294,7 +294,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Options for this are:
@@ -539,14 +539,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2008,7 +2008,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2033,7 +2033,7 @@
         <v>87.213999999999999</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>499</v>
       </c>
       <c r="C2" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
Added Basic Histogram Support
Program now outputs a histogram of the hydrogen amount used. Will add
flexibility later to output other things too.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -2008,7 +2008,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2033,7 +2033,7 @@
         <v>87.213999999999999</v>
       </c>
       <c r="B2">
-        <v>499</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
Must commit to pull
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -2014,7 +2014,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2044,7 +2044,7 @@
         <v>87.213999999999999</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>867</v>
       </c>
       <c r="C2" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
Added Variable histogram bar number
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -308,7 +308,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="74">
   <si>
     <t>Name</t>
   </si>
@@ -527,6 +527,9 @@
   </si>
   <si>
     <t>Total Cost</t>
+  </si>
+  <si>
+    <t>HistogramBars</t>
   </si>
 </sst>
 </file>
@@ -2011,10 +2014,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2025,7 +2028,7 @@
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -2038,13 +2041,16 @@
       <c r="D1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>87.213999999999999</v>
       </c>
       <c r="B2">
-        <v>867</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>70</v>
@@ -2052,13 +2058,16 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>17</v>
       </c>

</xml_diff>